<commit_message>
Added last completed labs
</commit_message>
<xml_diff>
--- a/Physics/4.3.1/4.3.1.xlsx
+++ b/Physics/4.3.1/4.3.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\4.3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE939AF-39FE-47F1-9390-3743A44B84B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE3AA4-45A6-4451-93CF-AEB9BE09B249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="16200" windowHeight="9970" xr2:uid="{0C18017D-60C2-42C9-AA29-6461B35D5045}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{0C18017D-60C2-42C9-AA29-6461B35D5045}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>S_2</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Меньше щель - меньше количество полос</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -444,15 +447,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BAC323-4C60-4692-9976-A233BB35A3E5}">
-  <dimension ref="A3:P20"/>
+  <dimension ref="A3:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -463,7 +470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -474,7 +481,7 @@
         <v>49.4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -490,14 +497,38 @@
       <c r="N5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P5">
+        <f>E6+1</f>
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <f>P5/2</f>
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <f>SQRT((49.4 - F6)/100 * Q5 * 546.1/1000000000)</f>
+        <v>9.9145347848499611E-5</v>
+      </c>
+      <c r="S5">
+        <f>2*R5</f>
+        <v>1.9829069569699922E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <v>47.6</v>
       </c>
+      <c r="H6">
+        <f xml:space="preserve"> SQRT((49.4 - F6)/100 * E6 * 5461/10000000000)</f>
+        <v>9.9145347848499611E-5</v>
+      </c>
+      <c r="I6">
+        <f>2*H6</f>
+        <v>1.9829069569699922E-4</v>
+      </c>
       <c r="J6" t="s">
         <v>4</v>
       </c>
@@ -507,8 +538,24 @@
       <c r="N6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P6">
+        <f t="shared" ref="P6:P11" si="0">E7+1</f>
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q10" si="1">P6/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R10" si="2">SQRT((49.4 - F7)/100 * Q6 * 546.1/1000000000)</f>
+        <v>9.9145347848499503E-5</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:S10" si="3">2*R6</f>
+        <v>1.9829069569699901E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -521,41 +568,137 @@
       <c r="F7">
         <v>48.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <f t="shared" ref="H7:H11" si="4" xml:space="preserve"> SQRT((49.4 - F7)/100 * E7 * 5461/10000000000)</f>
+        <v>1.1448318653846055E-4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I11" si="5">2*H7</f>
+        <v>2.289663730769211E-4</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>9.3475130382364107E-5</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>1.8695026076472821E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8">
         <v>48.6</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>1.1448318653846055E-4</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>2.289663730769211E-4</v>
+      </c>
       <c r="J8" t="s">
         <v>5</v>
       </c>
       <c r="N8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>9.0506905813866043E-5</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>1.8101381162773209E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9">
         <v>48.8</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>1.1448318653846087E-4</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>2.2896637307692175E-4</v>
+      </c>
       <c r="L9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>8.0951837533189928E-5</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>1.6190367506637986E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>1.0450837287031104E-4</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>2.0901674574062208E-4</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>7.57235102197458E-5</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>1.514470204394916E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>18</v>
       </c>
@@ -565,16 +708,88 @@
       <c r="F11">
         <v>49.1</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>9.9145347848499205E-5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>1.9829069569699841E-4</v>
+      </c>
       <c r="N11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K12">
+        <v>-2</v>
+      </c>
+      <c r="L12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>-1</v>
+      </c>
+      <c r="L13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I14">
+        <f>1000000*I6</f>
+        <v>198.29069569699922</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <f>(3.8 - 1.42) * 400</f>
+        <v>952</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I21" si="6">1000000*I7</f>
+        <v>228.96637307692109</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>106</v>
+      </c>
       <c r="N15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="13:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <f t="shared" si="6"/>
+        <v>228.96637307692109</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <f t="shared" si="6"/>
+        <v>228.96637307692174</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <f t="shared" si="6"/>
+        <v>209.01674574062207</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <f t="shared" si="6"/>
+        <v>198.2906956969984</v>
+      </c>
       <c r="M19" t="s">
         <v>14</v>
       </c>
@@ -588,7 +803,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="13:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <f>1.4 - 2.4</f>
+        <v>-1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="M20">
         <v>1.9</v>
       </c>
@@ -600,6 +823,176 @@
       </c>
       <c r="P20">
         <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24">
+        <f>212/1000000</f>
+        <v>2.12E-4</v>
+      </c>
+      <c r="I24">
+        <f>12.5/100*546.1/1000000000/G24</f>
+        <v>3.219929245283019E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="H26">
+        <v>-1</v>
+      </c>
+      <c r="I26">
+        <v>-0.3</v>
+      </c>
+      <c r="J26">
+        <v>0.4</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1.7</v>
+      </c>
+      <c r="M26">
+        <v>2.5</v>
+      </c>
+      <c r="N26">
+        <v>3</v>
+      </c>
+      <c r="O26">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <f>1.5 + D28</f>
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>-1</v>
+      </c>
+      <c r="E28">
+        <f>400*D28</f>
+        <v>-400</v>
+      </c>
+      <c r="F28">
+        <f>400*C28</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <f t="shared" ref="C29:C34" si="7">1.5 + D29</f>
+        <v>1.3</v>
+      </c>
+      <c r="D29">
+        <v>-0.2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E35" si="8">400*D29</f>
+        <v>-80</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:F34" si="9">400*C29</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <f t="shared" si="7"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D30">
+        <v>0.7</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="8"/>
+        <v>280</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="9"/>
+        <v>880.00000000000011</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <f t="shared" si="7"/>
+        <v>2.9</v>
+      </c>
+      <c r="D31">
+        <v>1.4</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="8"/>
+        <v>560</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="9"/>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <f t="shared" si="7"/>
+        <v>3.8</v>
+      </c>
+      <c r="D32">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="8"/>
+        <v>919.99999999999989</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="9"/>
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <f t="shared" si="7"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D33">
+        <v>3.1</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="8"/>
+        <v>1240</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="9"/>
+        <v>1839.9999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <f t="shared" si="7"/>
+        <v>5.3</v>
+      </c>
+      <c r="D34">
+        <v>3.8</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="8"/>
+        <v>1520</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="9"/>
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="E35">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>